<commit_message>
Files tot nu toe gebruikt
</commit_message>
<xml_diff>
--- a/DataPBAS.xlsx
+++ b/DataPBAS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sybra\Documents\GitHub\professional_business_analytics_skills\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D98C6338-BF57-48D2-80A6-F2F0542FCA6B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FA57BB-C5E3-490E-A6CF-1834E745D5DF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{9F4E300F-392D-41AA-9513-FB2EB37B5714}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="53">
   <si>
     <t>VGA</t>
   </si>
@@ -156,15 +156,9 @@
     <t>Substrate size</t>
   </si>
   <si>
-    <t>width</t>
-  </si>
-  <si>
     <t>m</t>
   </si>
   <si>
-    <t>height</t>
-  </si>
-  <si>
     <t>Tax rate</t>
   </si>
   <si>
@@ -190,6 +184,18 @@
   </si>
   <si>
     <t>Yieldpermarket</t>
+  </si>
+  <si>
+    <t>Cost Type</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Blanco</t>
+  </si>
+  <si>
+    <t>Blaco</t>
   </si>
 </sst>
 </file>
@@ -545,7 +551,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:J17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -567,13 +573,13 @@
         <v>17</v>
       </c>
       <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" t="s">
         <v>47</v>
-      </c>
-      <c r="E1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1721,9 +1727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE74EC4-8259-407A-BBEE-A2F32D4EEB7C}">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1731,6 +1735,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
       <c r="C1" t="s">
         <v>18</v>
       </c>
@@ -1894,12 +1904,21 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
       <c r="C1" t="s">
         <v>18</v>
       </c>
@@ -1975,13 +1994,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED897D7E-47F5-4242-AA61-4DF3F8F0F250}">
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
       </c>
       <c r="D1">
         <v>2003</v>
@@ -2185,143 +2215,147 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42A1901E-2D9E-49F6-A950-02FE45DAD9BD}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
       <c r="C1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="D2">
+      <c r="C2">
         <v>60000</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B3" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="1">
+      <c r="C3" s="1">
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>33</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B4" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="1">
+      <c r="C4" s="1">
         <v>0.04</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>34</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B5" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="1">
+      <c r="C5" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>36</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B6" t="s">
         <v>37</v>
       </c>
-      <c r="D6">
+      <c r="C6">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>38</v>
       </c>
       <c r="B7" t="s">
         <v>39</v>
       </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7">
+      <c r="C7">
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>38</v>
       </c>
       <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>41</v>
       </c>
-      <c r="C8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8">
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="C10">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>43</v>
       </c>
-      <c r="C10" t="s">
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>44</v>
       </c>
-      <c r="D10">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12">
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12">
         <v>30</v>
       </c>
     </row>

</xml_diff>